<commit_message>
added more country flags
</commit_message>
<xml_diff>
--- a/docs/flags.xlsx
+++ b/docs/flags.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COES" sheetId="5" r:id="rId1"/>
@@ -3985,7 +3985,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I142" sqref="I142"/>
     </sheetView>
@@ -17194,8 +17194,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C255"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A245" sqref="A5:A245"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17229,7 +17229,7 @@
         <v>Andorra</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>"{id:" &amp; CO!A3 &amp; ",code:""" &amp; CO!B3 &amp; """,name:""" &amp; CO!E3 &amp; """,x:" &amp; CO!G3&amp;"},"</f>
         <v>{id:1002,code:"AE",name:"Emiratos Árabes Unidos",x:0},</v>
@@ -17243,7 +17243,7 @@
         <v>United Arab Emirates</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>"{id:" &amp; CO!A4 &amp; ",code:""" &amp; CO!B4 &amp; """,name:""" &amp; CO!E4 &amp; """,x:" &amp; CO!G4&amp;"},"</f>
         <v>{id:1003,code:"AF",name:"Afganistán",x:0},</v>
@@ -17299,7 +17299,7 @@
         <v>Albania</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>"{id:" &amp; CO!A8 &amp; ",code:""" &amp; CO!B8 &amp; """,name:""" &amp; CO!E8 &amp; """,x:" &amp; CO!G8&amp;"},"</f>
         <v>{id:1007,code:"AM",name:"Armenia",x:0},</v>
@@ -17313,7 +17313,7 @@
         <v>Armenia</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>"{id:" &amp; CO!A9 &amp; ",code:""" &amp; CO!B9 &amp; """,name:""" &amp; CO!E9 &amp; """,x:" &amp; CO!G9&amp;"},"</f>
         <v>{id:1008,code:"AO",name:"Angola",x:0},</v>
@@ -17327,7 +17327,7 @@
         <v>Angola</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>"{id:" &amp; CO!A10 &amp; ",code:""" &amp; CO!B10 &amp; """,name:""" &amp; CO!E10 &amp; """,x:" &amp; CO!G10&amp;"},"</f>
         <v>{id:1009,code:"AQ",name:"Antártida",x:0},</v>
@@ -17425,7 +17425,7 @@
         <v>Âland Islands</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>"{id:" &amp; CO!A17 &amp; ",code:""" &amp; CO!B17 &amp; """,name:""" &amp; CO!E17 &amp; """,x:" &amp; CO!G17&amp;"},"</f>
         <v>{id:1016,code:"AZ",name:"Azerbayán",x:0},</v>
@@ -17467,7 +17467,7 @@
         <v>Barbados</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>"{id:" &amp; CO!A20 &amp; ",code:""" &amp; CO!B20 &amp; """,name:""" &amp; CO!E20 &amp; """,x:" &amp; CO!G20&amp;"},"</f>
         <v>{id:1019,code:"BD",name:"Bangladesh",x:0},</v>
@@ -17495,7 +17495,7 @@
         <v>Belgium</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>"{id:" &amp; CO!A22 &amp; ",code:""" &amp; CO!B22 &amp; """,name:""" &amp; CO!E22 &amp; """,x:" &amp; CO!G22&amp;"},"</f>
         <v>{id:1021,code:"BF",name:"Burkina Faso",x:0},</v>
@@ -17523,7 +17523,7 @@
         <v>Bulgaria</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>"{id:" &amp; CO!A24 &amp; ",code:""" &amp; CO!B24 &amp; """,name:""" &amp; CO!E24 &amp; """,x:" &amp; CO!G24&amp;"},"</f>
         <v>{id:1023,code:"BH",name:"Bahrein",x:0},</v>
@@ -17537,7 +17537,7 @@
         <v>Bahrain</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>"{id:" &amp; CO!A25 &amp; ",code:""" &amp; CO!B25 &amp; """,name:""" &amp; CO!E25 &amp; """,x:" &amp; CO!G25&amp;"},"</f>
         <v>{id:1024,code:"BI",name:"Burundi",x:0},</v>
@@ -17551,7 +17551,7 @@
         <v>Burundi</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>"{id:" &amp; CO!A26 &amp; ",code:""" &amp; CO!B26 &amp; """,name:""" &amp; CO!E26 &amp; """,x:" &amp; CO!G26&amp;"},"</f>
         <v>{id:1025,code:"BJ",name:"Benín",x:0},</v>
@@ -17593,7 +17593,7 @@
         <v>Bermuda</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>"{id:" &amp; CO!A29 &amp; ",code:""" &amp; CO!B29 &amp; """,name:""" &amp; CO!E29 &amp; """,x:" &amp; CO!G29&amp;"},"</f>
         <v>{id:1028,code:"BN",name:"Brunái",x:0},</v>
@@ -17663,7 +17663,7 @@
         <v>Bahamas</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>"{id:" &amp; CO!A34 &amp; ",code:""" &amp; CO!B34 &amp; """,name:""" &amp; CO!E34 &amp; """,x:" &amp; CO!G34&amp;"},"</f>
         <v>{id:1033,code:"BT",name:"Bhután",x:0},</v>
@@ -17691,7 +17691,7 @@
         <v>Bouvet Island</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>"{id:" &amp; CO!A36 &amp; ",code:""" &amp; CO!B36 &amp; """,name:""" &amp; CO!E36 &amp; """,x:" &amp; CO!G36&amp;"},"</f>
         <v>{id:1035,code:"BW",name:"Botsuana",x:0},</v>
@@ -17761,7 +17761,7 @@
         <v>Cocos (Keeling) Islands</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>"{id:" &amp; CO!A41 &amp; ",code:""" &amp; CO!B41 &amp; """,name:""" &amp; CO!E41 &amp; """,x:" &amp; CO!G41&amp;"},"</f>
         <v>{id:1040,code:"CD",name:"República Democrática del Congo",x:0},</v>
@@ -17775,7 +17775,7 @@
         <v>Congo</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>"{id:" &amp; CO!A42 &amp; ",code:""" &amp; CO!B42 &amp; """,name:""" &amp; CO!E42 &amp; """,x:" &amp; CO!G42&amp;"},"</f>
         <v>{id:1041,code:"CF",name:"República Centroafricana",x:0},</v>
@@ -17789,7 +17789,7 @@
         <v>Central African Republic</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>"{id:" &amp; CO!A43 &amp; ",code:""" &amp; CO!B43 &amp; """,name:""" &amp; CO!E43 &amp; """,x:" &amp; CO!G43&amp;"},"</f>
         <v>{id:1042,code:"CG",name:"República del Congo",x:0},</v>
@@ -17817,7 +17817,7 @@
         <v>Switzerland</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>"{id:" &amp; CO!A45 &amp; ",code:""" &amp; CO!B45 &amp; """,name:""" &amp; CO!E45 &amp; """,x:" &amp; CO!G45&amp;"},"</f>
         <v>{id:1044,code:"CI",name:"Costa de Marfil",x:0},</v>
@@ -17859,7 +17859,7 @@
         <v>Chile</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>"{id:" &amp; CO!A48 &amp; ",code:""" &amp; CO!B48 &amp; """,name:""" &amp; CO!E48 &amp; """,x:" &amp; CO!G48&amp;"},"</f>
         <v>{id:1047,code:"CM",name:"Camerún",x:0},</v>
@@ -17873,7 +17873,7 @@
         <v>Cameroon</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>"{id:" &amp; CO!A49 &amp; ",code:""" &amp; CO!B49 &amp; """,name:""" &amp; CO!E49 &amp; """,x:" &amp; CO!G49&amp;"},"</f>
         <v>{id:1048,code:"CN",name:"China",x:0},</v>
@@ -17929,7 +17929,7 @@
         <v>Cuba</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>"{id:" &amp; CO!A53 &amp; ",code:""" &amp; CO!B53 &amp; """,name:""" &amp; CO!E53 &amp; """,x:" &amp; CO!G53&amp;"},"</f>
         <v>{id:1052,code:"CV",name:"Cabo Verde",x:0},</v>
@@ -18013,7 +18013,7 @@
         <v>Germany</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>"{id:" &amp; CO!A59 &amp; ",code:""" &amp; CO!B59 &amp; """,name:""" &amp; CO!E59 &amp; """,x:" &amp; CO!G59&amp;"},"</f>
         <v>{id:1058,code:"DJ",name:"Yibuti",x:0},</v>
@@ -18069,7 +18069,7 @@
         <v>Dominican Republic</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>"{id:" &amp; CO!A63 &amp; ",code:""" &amp; CO!B63 &amp; """,name:""" &amp; CO!E63 &amp; """,x:" &amp; CO!G63&amp;"},"</f>
         <v>{id:1062,code:"DZ",name:"Algeria",x:0},</v>
@@ -18111,7 +18111,7 @@
         <v>Estonia</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>"{id:" &amp; CO!A66 &amp; ",code:""" &amp; CO!B66 &amp; """,name:""" &amp; CO!E66 &amp; """,x:" &amp; CO!G66&amp;"},"</f>
         <v>{id:1065,code:"EG",name:"Egipto",x:0},</v>
@@ -18125,7 +18125,7 @@
         <v>Egypt</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>"{id:" &amp; CO!A67 &amp; ",code:""" &amp; CO!B67 &amp; """,name:""" &amp; CO!E67 &amp; """,x:" &amp; CO!G67&amp;"},"</f>
         <v>{id:1066,code:"EH",name:"Sahara Occidental",x:0},</v>
@@ -18139,7 +18139,7 @@
         <v>Western Sahara</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>"{id:" &amp; CO!A68 &amp; ",code:""" &amp; CO!B68 &amp; """,name:""" &amp; CO!E68 &amp; """,x:" &amp; CO!G68&amp;"},"</f>
         <v>{id:1067,code:"ER",name:"Eritrea",x:0},</v>
@@ -18167,7 +18167,7 @@
         <v>Spain</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>"{id:" &amp; CO!A70 &amp; ",code:""" &amp; CO!B70 &amp; """,name:""" &amp; CO!E70 &amp; """,x:" &amp; CO!G70&amp;"},"</f>
         <v>{id:1069,code:"ET",name:"Etiopía",x:0},</v>
@@ -18265,7 +18265,7 @@
         <v>France</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>"{id:" &amp; CO!A77 &amp; ",code:""" &amp; CO!B77 &amp; """,name:""" &amp; CO!E77 &amp; """,x:" &amp; CO!G77&amp;"},"</f>
         <v>{id:1076,code:"GA",name:"Gabón",x:0},</v>
@@ -18279,7 +18279,7 @@
         <v>Gabon</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>"{id:" &amp; CO!A78 &amp; ",code:""" &amp; CO!B78 &amp; """,name:""" &amp; CO!E78 &amp; """,x:" &amp; CO!G78&amp;"},"</f>
         <v>{id:1077,code:"GB-ENG",name:"Inglaterra",x:0},</v>
@@ -18293,7 +18293,7 @@
         <v>England</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>"{id:" &amp; CO!A79 &amp; ",code:""" &amp; CO!B79 &amp; """,name:""" &amp; CO!E79 &amp; """,x:" &amp; CO!G79&amp;"},"</f>
         <v>{id:1078,code:"GB-NIR",name:"Irlanda del Norte",x:0},</v>
@@ -18307,7 +18307,7 @@
         <v>Northern Ireland</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>"{id:" &amp; CO!A80 &amp; ",code:""" &amp; CO!B80 &amp; """,name:""" &amp; CO!E80 &amp; """,x:" &amp; CO!G80&amp;"},"</f>
         <v>{id:1079,code:"GB-SCT",name:"Escocia",x:0},</v>
@@ -18321,7 +18321,7 @@
         <v>Scotland</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f>"{id:" &amp; CO!A81 &amp; ",code:""" &amp; CO!B81 &amp; """,name:""" &amp; CO!E81 &amp; """,x:" &amp; CO!G81&amp;"},"</f>
         <v>{id:1080,code:"GB-WLS",name:"Gales",x:0},</v>
@@ -18363,7 +18363,7 @@
         <v>Grenada</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>"{id:" &amp; CO!A84 &amp; ",code:""" &amp; CO!B84 &amp; """,name:""" &amp; CO!E84 &amp; """,x:" &amp; CO!G84&amp;"},"</f>
         <v>{id:1083,code:"GE",name:"Georgia",x:0},</v>
@@ -18405,7 +18405,7 @@
         <v>Guernsey</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>"{id:" &amp; CO!A87 &amp; ",code:""" &amp; CO!B87 &amp; """,name:""" &amp; CO!E87 &amp; """,x:" &amp; CO!G87&amp;"},"</f>
         <v>{id:1086,code:"GH",name:"Ghana",x:0},</v>
@@ -18447,7 +18447,7 @@
         <v>Greenland</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f>"{id:" &amp; CO!A90 &amp; ",code:""" &amp; CO!B90 &amp; """,name:""" &amp; CO!E90 &amp; """,x:" &amp; CO!G90&amp;"},"</f>
         <v>{id:1089,code:"GM",name:"Gambia",x:0},</v>
@@ -18461,7 +18461,7 @@
         <v>Gambia</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f>"{id:" &amp; CO!A91 &amp; ",code:""" &amp; CO!B91 &amp; """,name:""" &amp; CO!E91 &amp; """,x:" &amp; CO!G91&amp;"},"</f>
         <v>{id:1090,code:"GN",name:"Guinea",x:0},</v>
@@ -18489,7 +18489,7 @@
         <v>Guadeloupe</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>"{id:" &amp; CO!A93 &amp; ",code:""" &amp; CO!B93 &amp; """,name:""" &amp; CO!E93 &amp; """,x:" &amp; CO!G93&amp;"},"</f>
         <v>{id:1092,code:"GQ",name:"Guinea Ecuatorial",x:0},</v>
@@ -18559,7 +18559,7 @@
         <v>Guam</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>"{id:" &amp; CO!A98 &amp; ",code:""" &amp; CO!B98 &amp; """,name:""" &amp; CO!E98 &amp; """,x:" &amp; CO!G98&amp;"},"</f>
         <v>{id:1097,code:"GW",name:"Guinea-Bissau",x:0},</v>
@@ -18587,7 +18587,7 @@
         <v>Guyana</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f>"{id:" &amp; CO!A100 &amp; ",code:""" &amp; CO!B100 &amp; """,name:""" &amp; CO!E100 &amp; """,x:" &amp; CO!G100&amp;"},"</f>
         <v>{id:1099,code:"HK",name:"Hong kong",x:0},</v>
@@ -18671,7 +18671,7 @@
         <v>Hungary</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
         <f>"{id:" &amp; CO!A106 &amp; ",code:""" &amp; CO!B106 &amp; """,name:""" &amp; CO!E106 &amp; """,x:" &amp; CO!G106&amp;"},"</f>
         <v>{id:1105,code:"ID",name:"Indonesia",x:0},</v>
@@ -18699,7 +18699,7 @@
         <v>Ireland</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
         <f>"{id:" &amp; CO!A108 &amp; ",code:""" &amp; CO!B108 &amp; """,name:""" &amp; CO!E108 &amp; """,x:" &amp; CO!G108&amp;"},"</f>
         <v>{id:1107,code:"IL",name:"Israel",x:0},</v>
@@ -18727,7 +18727,7 @@
         <v>Isle of Man</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
         <f>"{id:" &amp; CO!A110 &amp; ",code:""" &amp; CO!B110 &amp; """,name:""" &amp; CO!E110 &amp; """,x:" &amp; CO!G110&amp;"},"</f>
         <v>{id:1109,code:"IN",name:"India",x:0},</v>
@@ -18755,7 +18755,7 @@
         <v>British Indian Ocean Territory</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
         <f>"{id:" &amp; CO!A112 &amp; ",code:""" &amp; CO!B112 &amp; """,name:""" &amp; CO!E112 &amp; """,x:" &amp; CO!G112&amp;"},"</f>
         <v>{id:1111,code:"IQ",name:"Irak",x:0},</v>
@@ -18769,7 +18769,7 @@
         <v>Iraq</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
         <f>"{id:" &amp; CO!A113 &amp; ",code:""" &amp; CO!B113 &amp; """,name:""" &amp; CO!E113 &amp; """,x:" &amp; CO!G113&amp;"},"</f>
         <v>{id:1112,code:"IR",name:"Irán",x:0},</v>
@@ -18839,7 +18839,7 @@
         <v>Jamaica</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
         <f>"{id:" &amp; CO!A118 &amp; ",code:""" &amp; CO!B118 &amp; """,name:""" &amp; CO!E118 &amp; """,x:" &amp; CO!G118&amp;"},"</f>
         <v>{id:1117,code:"JO",name:"Jordania",x:0},</v>
@@ -18853,7 +18853,7 @@
         <v>Jordan</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
         <f>"{id:" &amp; CO!A119 &amp; ",code:""" &amp; CO!B119 &amp; """,name:""" &amp; CO!E119 &amp; """,x:" &amp; CO!G119&amp;"},"</f>
         <v>{id:1118,code:"JP",name:"Japón",x:0},</v>
@@ -18867,7 +18867,7 @@
         <v>Japan</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
         <f>"{id:" &amp; CO!A120 &amp; ",code:""" &amp; CO!B120 &amp; """,name:""" &amp; CO!E120 &amp; """,x:" &amp; CO!G120&amp;"},"</f>
         <v>{id:1119,code:"KE",name:"Kenia",x:0},</v>
@@ -18881,7 +18881,7 @@
         <v>Kenya</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
         <f>"{id:" &amp; CO!A121 &amp; ",code:""" &amp; CO!B121 &amp; """,name:""" &amp; CO!E121 &amp; """,x:" &amp; CO!G121&amp;"},"</f>
         <v>{id:1120,code:"KG",name:"Kirgizstán",x:0},</v>
@@ -18895,7 +18895,7 @@
         <v>Kyrgyzstan</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
         <f>"{id:" &amp; CO!A122 &amp; ",code:""" &amp; CO!B122 &amp; """,name:""" &amp; CO!E122 &amp; """,x:" &amp; CO!G122&amp;"},"</f>
         <v>{id:1121,code:"KH",name:"Camboya",x:0},</v>
@@ -18923,7 +18923,7 @@
         <v>Kiribati</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
         <f>"{id:" &amp; CO!A124 &amp; ",code:""" &amp; CO!B124 &amp; """,name:""" &amp; CO!E124 &amp; """,x:" &amp; CO!G124&amp;"},"</f>
         <v>{id:1123,code:"KM",name:"Comoras",x:0},</v>
@@ -18951,7 +18951,7 @@
         <v>Saint Kitts and Nevis</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
         <f>"{id:" &amp; CO!A126 &amp; ",code:""" &amp; CO!B126 &amp; """,name:""" &amp; CO!E126 &amp; """,x:" &amp; CO!G126&amp;"},"</f>
         <v>{id:1125,code:"KP",name:"Corea del Norte",x:0},</v>
@@ -18965,7 +18965,7 @@
         <v>Korea</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
         <f>"{id:" &amp; CO!A127 &amp; ",code:""" &amp; CO!B127 &amp; """,name:""" &amp; CO!E127 &amp; """,x:" &amp; CO!G127&amp;"},"</f>
         <v>{id:1126,code:"KR",name:"Corea del Sur",x:0},</v>
@@ -18979,7 +18979,7 @@
         <v>Korea</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
         <f>"{id:" &amp; CO!A128 &amp; ",code:""" &amp; CO!B128 &amp; """,name:""" &amp; CO!E128 &amp; """,x:" &amp; CO!G128&amp;"},"</f>
         <v>{id:1127,code:"KW",name:"Kuwait",x:0},</v>
@@ -19007,7 +19007,7 @@
         <v>Cayman Islands</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
         <f>"{id:" &amp; CO!A130 &amp; ",code:""" &amp; CO!B130 &amp; """,name:""" &amp; CO!E130 &amp; """,x:" &amp; CO!G130&amp;"},"</f>
         <v>{id:1129,code:"KZ",name:"Kazajistán",x:0},</v>
@@ -19021,7 +19021,7 @@
         <v>Kazakhstan</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f>"{id:" &amp; CO!A131 &amp; ",code:""" &amp; CO!B131 &amp; """,name:""" &amp; CO!E131 &amp; """,x:" &amp; CO!G131&amp;"},"</f>
         <v>{id:1130,code:"LA",name:"Laos",x:0},</v>
@@ -19035,7 +19035,7 @@
         <v>Lao People's Democratic Republic</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
         <f>"{id:" &amp; CO!A132 &amp; ",code:""" &amp; CO!B132 &amp; """,name:""" &amp; CO!E132 &amp; """,x:" &amp; CO!G132&amp;"},"</f>
         <v>{id:1131,code:"LB",name:"Líbano",x:0},</v>
@@ -19077,7 +19077,7 @@
         <v>Liechtenstein</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
         <f>"{id:" &amp; CO!A135 &amp; ",code:""" &amp; CO!B135 &amp; """,name:""" &amp; CO!E135 &amp; """,x:" &amp; CO!G135&amp;"},"</f>
         <v>{id:1134,code:"LK",name:"Sri lanka",x:0},</v>
@@ -19091,7 +19091,7 @@
         <v>Sri Lanka</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
         <f>"{id:" &amp; CO!A136 &amp; ",code:""" &amp; CO!B136 &amp; """,name:""" &amp; CO!E136 &amp; """,x:" &amp; CO!G136&amp;"},"</f>
         <v>{id:1135,code:"LR",name:"Liberia",x:0},</v>
@@ -19105,7 +19105,7 @@
         <v>Liberia</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
         <f>"{id:" &amp; CO!A137 &amp; ",code:""" &amp; CO!B137 &amp; """,name:""" &amp; CO!E137 &amp; """,x:" &amp; CO!G137&amp;"},"</f>
         <v>{id:1136,code:"LS",name:"Lesoto",x:0},</v>
@@ -19161,7 +19161,7 @@
         <v>Latvia</v>
       </c>
     </row>
-    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
         <f>"{id:" &amp; CO!A141 &amp; ",code:""" &amp; CO!B141 &amp; """,name:""" &amp; CO!E141 &amp; """,x:" &amp; CO!G141&amp;"},"</f>
         <v>{id:1140,code:"LY",name:"Libia",x:0},</v>
@@ -19175,7 +19175,7 @@
         <v>Libya</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
         <f>"{id:" &amp; CO!A142 &amp; ",code:""" &amp; CO!B142 &amp; """,name:""" &amp; CO!E142 &amp; """,x:" &amp; CO!G142&amp;"},"</f>
         <v>{id:1141,code:"MA",name:"Marruecos",x:0},</v>
@@ -19245,7 +19245,7 @@
         <v>Saint Martin</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f>"{id:" &amp; CO!A147 &amp; ",code:""" &amp; CO!B147 &amp; """,name:""" &amp; CO!E147 &amp; """,x:" &amp; CO!G147&amp;"},"</f>
         <v>{id:1146,code:"MG",name:"Madagascar",x:0},</v>
@@ -19287,7 +19287,7 @@
         <v>Macedonia</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
         <f>"{id:" &amp; CO!A150 &amp; ",code:""" &amp; CO!B150 &amp; """,name:""" &amp; CO!E150 &amp; """,x:" &amp; CO!G150&amp;"},"</f>
         <v>{id:1149,code:"ML",name:"Mali",x:0},</v>
@@ -19301,7 +19301,7 @@
         <v>Mali</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
         <f>"{id:" &amp; CO!A151 &amp; ",code:""" &amp; CO!B151 &amp; """,name:""" &amp; CO!E151 &amp; """,x:" &amp; CO!G151&amp;"},"</f>
         <v>{id:1150,code:"MM",name:"Birmania",x:0},</v>
@@ -19315,7 +19315,7 @@
         <v>Myanmar</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
         <f>"{id:" &amp; CO!A152 &amp; ",code:""" &amp; CO!B152 &amp; """,name:""" &amp; CO!E152 &amp; """,x:" &amp; CO!G152&amp;"},"</f>
         <v>{id:1151,code:"MN",name:"Mongolia",x:0},</v>
@@ -19371,7 +19371,7 @@
         <v>Martinique</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
         <f>"{id:" &amp; CO!A156 &amp; ",code:""" &amp; CO!B156 &amp; """,name:""" &amp; CO!E156 &amp; """,x:" &amp; CO!G156&amp;"},"</f>
         <v>{id:1155,code:"MR",name:"Mauritania",x:0},</v>
@@ -19413,7 +19413,7 @@
         <v>Malta</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
         <f>"{id:" &amp; CO!A159 &amp; ",code:""" &amp; CO!B159 &amp; """,name:""" &amp; CO!E159 &amp; """,x:" &amp; CO!G159&amp;"},"</f>
         <v>{id:1158,code:"MU",name:"Mauricio",x:0},</v>
@@ -19441,7 +19441,7 @@
         <v>Maldives</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
         <f>"{id:" &amp; CO!A161 &amp; ",code:""" &amp; CO!B161 &amp; """,name:""" &amp; CO!E161 &amp; """,x:" &amp; CO!G161&amp;"},"</f>
         <v>{id:1160,code:"MW",name:"Malawi",x:0},</v>
@@ -19469,7 +19469,7 @@
         <v>Mexico</v>
       </c>
     </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
         <f>"{id:" &amp; CO!A163 &amp; ",code:""" &amp; CO!B163 &amp; """,name:""" &amp; CO!E163 &amp; """,x:" &amp; CO!G163&amp;"},"</f>
         <v>{id:1162,code:"MY",name:"Malasia",x:0},</v>
@@ -19483,7 +19483,7 @@
         <v>Malaysia</v>
       </c>
     </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
         <f>"{id:" &amp; CO!A164 &amp; ",code:""" &amp; CO!B164 &amp; """,name:""" &amp; CO!E164 &amp; """,x:" &amp; CO!G164&amp;"},"</f>
         <v>{id:1163,code:"MZ",name:"Mozambique",x:0},</v>
@@ -19497,7 +19497,7 @@
         <v>Mozambique</v>
       </c>
     </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="str">
         <f>"{id:" &amp; CO!A165 &amp; ",code:""" &amp; CO!B165 &amp; """,name:""" &amp; CO!E165 &amp; """,x:" &amp; CO!G165&amp;"},"</f>
         <v>{id:1164,code:"NA",name:"Namibia",x:0},</v>
@@ -19525,7 +19525,7 @@
         <v>New Caledonia</v>
       </c>
     </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="str">
         <f>"{id:" &amp; CO!A167 &amp; ",code:""" &amp; CO!B167 &amp; """,name:""" &amp; CO!E167 &amp; """,x:" &amp; CO!G167&amp;"},"</f>
         <v>{id:1166,code:"NE",name:"Niger",x:0},</v>
@@ -19553,7 +19553,7 @@
         <v>Norfolk Island</v>
       </c>
     </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
         <f>"{id:" &amp; CO!A169 &amp; ",code:""" &amp; CO!B169 &amp; """,name:""" &amp; CO!E169 &amp; """,x:" &amp; CO!G169&amp;"},"</f>
         <v>{id:1168,code:"NG",name:"Nigeria",x:0},</v>
@@ -19609,7 +19609,7 @@
         <v>Norway</v>
       </c>
     </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="str">
         <f>"{id:" &amp; CO!A173 &amp; ",code:""" &amp; CO!B173 &amp; """,name:""" &amp; CO!E173 &amp; """,x:" &amp; CO!G173&amp;"},"</f>
         <v>{id:1172,code:"NP",name:"Nepal",x:0},</v>
@@ -19665,7 +19665,7 @@
         <v>New Zealand</v>
       </c>
     </row>
-    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
         <f>"{id:" &amp; CO!A177 &amp; ",code:""" &amp; CO!B177 &amp; """,name:""" &amp; CO!E177 &amp; """,x:" &amp; CO!G177&amp;"},"</f>
         <v>{id:1176,code:"OM",name:"Omán",x:0},</v>
@@ -19735,7 +19735,7 @@
         <v>Papua New Guinea</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="str">
         <f>"{id:" &amp; CO!A182 &amp; ",code:""" &amp; CO!B182 &amp; """,name:""" &amp; CO!E182 &amp; """,x:" &amp; CO!G182&amp;"},"</f>
         <v>{id:1181,code:"PH",name:"Filipinas",x:0},</v>
@@ -19749,7 +19749,7 @@
         <v>Philippines</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="str">
         <f>"{id:" &amp; CO!A183 &amp; ",code:""" &amp; CO!B183 &amp; """,name:""" &amp; CO!E183 &amp; """,x:" &amp; CO!G183&amp;"},"</f>
         <v>{id:1182,code:"PK",name:"Pakistán",x:0},</v>
@@ -19819,7 +19819,7 @@
         <v>Puerto Rico</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="str">
         <f>"{id:" &amp; CO!A188 &amp; ",code:""" &amp; CO!B188 &amp; """,name:""" &amp; CO!E188 &amp; """,x:" &amp; CO!G188&amp;"},"</f>
         <v>{id:1187,code:"PS",name:"Palestina",x:0},</v>
@@ -19875,7 +19875,7 @@
         <v>Paraguay</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="str">
         <f>"{id:" &amp; CO!A192 &amp; ",code:""" &amp; CO!B192 &amp; """,name:""" &amp; CO!E192 &amp; """,x:" &amp; CO!G192&amp;"},"</f>
         <v>{id:1191,code:"QA",name:"Qatar",x:0},</v>
@@ -19931,7 +19931,7 @@
         <v>Serbia</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="str">
         <f>"{id:" &amp; CO!A196 &amp; ",code:""" &amp; CO!B196 &amp; """,name:""" &amp; CO!E196 &amp; """,x:" &amp; CO!G196&amp;"},"</f>
         <v>{id:1195,code:"RU",name:"Rusia",x:0},</v>
@@ -19945,7 +19945,7 @@
         <v>Russian Federation</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="str">
         <f>"{id:" &amp; CO!A197 &amp; ",code:""" &amp; CO!B197 &amp; """,name:""" &amp; CO!E197 &amp; """,x:" &amp; CO!G197&amp;"},"</f>
         <v>{id:1196,code:"RW",name:"Ruanda",x:0},</v>
@@ -19959,7 +19959,7 @@
         <v>Rwanda</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="str">
         <f>"{id:" &amp; CO!A198 &amp; ",code:""" &amp; CO!B198 &amp; """,name:""" &amp; CO!E198 &amp; """,x:" &amp; CO!G198&amp;"},"</f>
         <v>{id:1197,code:"SA",name:"Arabia Saudita",x:0},</v>
@@ -19987,7 +19987,7 @@
         <v>Solomon Islands</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="str">
         <f>"{id:" &amp; CO!A200 &amp; ",code:""" &amp; CO!B200 &amp; """,name:""" &amp; CO!E200 &amp; """,x:" &amp; CO!G200&amp;"},"</f>
         <v>{id:1199,code:"SC",name:"Seychelles",x:0},</v>
@@ -20001,7 +20001,7 @@
         <v>Seychelles</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="str">
         <f>"{id:" &amp; CO!A201 &amp; ",code:""" &amp; CO!B201 &amp; """,name:""" &amp; CO!E201 &amp; """,x:" &amp; CO!G201&amp;"},"</f>
         <v>{id:1200,code:"SD",name:"Sudán",x:0},</v>
@@ -20029,7 +20029,7 @@
         <v>Sweden</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="str">
         <f>"{id:" &amp; CO!A203 &amp; ",code:""" &amp; CO!B203 &amp; """,name:""" &amp; CO!E203 &amp; """,x:" &amp; CO!G203&amp;"},"</f>
         <v>{id:1202,code:"SG",name:"Singapur",x:0},</v>
@@ -20099,7 +20099,7 @@
         <v>Slovakia</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="str">
         <f>"{id:" &amp; CO!A208 &amp; ",code:""" &amp; CO!B208 &amp; """,name:""" &amp; CO!E208 &amp; """,x:" &amp; CO!G208&amp;"},"</f>
         <v>{id:1207,code:"SL",name:"Sierra Leona",x:0},</v>
@@ -20127,7 +20127,7 @@
         <v>San Marino</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="str">
         <f>"{id:" &amp; CO!A210 &amp; ",code:""" &amp; CO!B210 &amp; """,name:""" &amp; CO!E210 &amp; """,x:" &amp; CO!G210&amp;"},"</f>
         <v>{id:1209,code:"SN",name:"Senegal",x:0},</v>
@@ -20141,7 +20141,7 @@
         <v>Senegal</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="str">
         <f>"{id:" &amp; CO!A211 &amp; ",code:""" &amp; CO!B211 &amp; """,name:""" &amp; CO!E211 &amp; """,x:" &amp; CO!G211&amp;"},"</f>
         <v>{id:1210,code:"SO",name:"Somalia",x:0},</v>
@@ -20169,7 +20169,7 @@
         <v>Suriname</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="str">
         <f>"{id:" &amp; CO!A213 &amp; ",code:""" &amp; CO!B213 &amp; """,name:""" &amp; CO!E213 &amp; """,x:" &amp; CO!G213&amp;"},"</f>
         <v>{id:1212,code:"SS",name:"Sudán del Sur",x:0},</v>
@@ -20183,7 +20183,7 @@
         <v>South Sudan</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="str">
         <f>"{id:" &amp; CO!A214 &amp; ",code:""" &amp; CO!B214 &amp; """,name:""" &amp; CO!E214 &amp; """,x:" &amp; CO!G214&amp;"},"</f>
         <v>{id:1213,code:"ST",name:"Santo Tomé y Príncipe",x:0},</v>
@@ -20225,7 +20225,7 @@
         <v>Sint Maarten (Dutch part)</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="str">
         <f>"{id:" &amp; CO!A217 &amp; ",code:""" &amp; CO!B217 &amp; """,name:""" &amp; CO!E217 &amp; """,x:" &amp; CO!G217&amp;"},"</f>
         <v>{id:1216,code:"SY",name:"Siria",x:0},</v>
@@ -20239,7 +20239,7 @@
         <v>Syrian Arab Republic</v>
       </c>
     </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="str">
         <f>"{id:" &amp; CO!A218 &amp; ",code:""" &amp; CO!B218 &amp; """,name:""" &amp; CO!E218 &amp; """,x:" &amp; CO!G218&amp;"},"</f>
         <v>{id:1217,code:"SZ",name:"Swazilandia",x:0},</v>
@@ -20267,7 +20267,7 @@
         <v>Turks and Caicos Islands</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="str">
         <f>"{id:" &amp; CO!A220 &amp; ",code:""" &amp; CO!B220 &amp; """,name:""" &amp; CO!E220 &amp; """,x:" &amp; CO!G220&amp;"},"</f>
         <v>{id:1219,code:"TD",name:"Chad",x:0},</v>
@@ -20295,7 +20295,7 @@
         <v>French Southern Territories</v>
       </c>
     </row>
-    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="str">
         <f>"{id:" &amp; CO!A222 &amp; ",code:""" &amp; CO!B222 &amp; """,name:""" &amp; CO!E222 &amp; """,x:" &amp; CO!G222&amp;"},"</f>
         <v>{id:1221,code:"TG",name:"Togo",x:0},</v>
@@ -20309,7 +20309,7 @@
         <v>Togo</v>
       </c>
     </row>
-    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="str">
         <f>"{id:" &amp; CO!A223 &amp; ",code:""" &amp; CO!B223 &amp; """,name:""" &amp; CO!E223 &amp; """,x:" &amp; CO!G223&amp;"},"</f>
         <v>{id:1222,code:"TH",name:"Tailandia",x:0},</v>
@@ -20323,7 +20323,7 @@
         <v>Thailand</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="str">
         <f>"{id:" &amp; CO!A224 &amp; ",code:""" &amp; CO!B224 &amp; """,name:""" &amp; CO!E224 &amp; """,x:" &amp; CO!G224&amp;"},"</f>
         <v>{id:1223,code:"TJ",name:"Tadjikistán",x:0},</v>
@@ -20351,7 +20351,7 @@
         <v>Tokelau</v>
       </c>
     </row>
-    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="str">
         <f>"{id:" &amp; CO!A226 &amp; ",code:""" &amp; CO!B226 &amp; """,name:""" &amp; CO!E226 &amp; """,x:" &amp; CO!G226&amp;"},"</f>
         <v>{id:1225,code:"TL",name:"Timor Oriental",x:0},</v>
@@ -20365,7 +20365,7 @@
         <v>Timor-Leste</v>
       </c>
     </row>
-    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="str">
         <f>"{id:" &amp; CO!A227 &amp; ",code:""" &amp; CO!B227 &amp; """,name:""" &amp; CO!E227 &amp; """,x:" &amp; CO!G227&amp;"},"</f>
         <v>{id:1226,code:"TM",name:"Turkmenistán",x:0},</v>
@@ -20379,7 +20379,7 @@
         <v>Turkmenistan</v>
       </c>
     </row>
-    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="str">
         <f>"{id:" &amp; CO!A228 &amp; ",code:""" &amp; CO!B228 &amp; """,name:""" &amp; CO!E228 &amp; """,x:" &amp; CO!G228&amp;"},"</f>
         <v>{id:1227,code:"TN",name:"Tunez",x:0},</v>
@@ -20407,7 +20407,7 @@
         <v>Tonga</v>
       </c>
     </row>
-    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="str">
         <f>"{id:" &amp; CO!A230 &amp; ",code:""" &amp; CO!B230 &amp; """,name:""" &amp; CO!E230 &amp; """,x:" &amp; CO!G230&amp;"},"</f>
         <v>{id:1229,code:"TR",name:"Turquía",x:0},</v>
@@ -20449,7 +20449,7 @@
         <v>Tuvalu</v>
       </c>
     </row>
-    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="str">
         <f>"{id:" &amp; CO!A233 &amp; ",code:""" &amp; CO!B233 &amp; """,name:""" &amp; CO!E233 &amp; """,x:" &amp; CO!G233&amp;"},"</f>
         <v>{id:1232,code:"TW",name:"Taiwán",x:0},</v>
@@ -20463,7 +20463,7 @@
         <v>Taiwan</v>
       </c>
     </row>
-    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="str">
         <f>"{id:" &amp; CO!A234 &amp; ",code:""" &amp; CO!B234 &amp; """,name:""" &amp; CO!E234 &amp; """,x:" &amp; CO!G234&amp;"},"</f>
         <v>{id:1233,code:"TZ",name:"Tanzania",x:0},</v>
@@ -20491,7 +20491,7 @@
         <v>Ukraine</v>
       </c>
     </row>
-    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="str">
         <f>"{id:" &amp; CO!A236 &amp; ",code:""" &amp; CO!B236 &amp; """,name:""" &amp; CO!E236 &amp; """,x:" &amp; CO!G236&amp;"},"</f>
         <v>{id:1235,code:"UG",name:"Uganda",x:0},</v>
@@ -20547,7 +20547,7 @@
         <v>Uruguay</v>
       </c>
     </row>
-    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="str">
         <f>"{id:" &amp; CO!A240 &amp; ",code:""" &amp; CO!B240 &amp; """,name:""" &amp; CO!E240 &amp; """,x:" &amp; CO!G240&amp;"},"</f>
         <v>{id:1239,code:"UZ",name:"Uzbekistán",x:0},</v>
@@ -20631,7 +20631,7 @@
         <v>US Virgin Islands</v>
       </c>
     </row>
-    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="str">
         <f>"{id:" &amp; CO!A246 &amp; ",code:""" &amp; CO!B246 &amp; """,name:""" &amp; CO!E246 &amp; """,x:" &amp; CO!G246&amp;"},"</f>
         <v>{id:1245,code:"VN",name:"Vietnam",x:0},</v>
@@ -20673,7 +20673,7 @@
         <v>Wallis and Futuna Islands</v>
       </c>
     </row>
-    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="str">
         <f>"{id:" &amp; CO!A249 &amp; ",code:""" &amp; CO!B249 &amp; """,name:""" &amp; CO!E249 &amp; """,x:" &amp; CO!G249&amp;"},"</f>
         <v>{id:1248,code:"XK",name:"Kósovo",x:0},</v>
@@ -20701,7 +20701,7 @@
         <v>Samoa</v>
       </c>
     </row>
-    <row r="251" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="str">
         <f>"{id:" &amp; CO!A251 &amp; ",code:""" &amp; CO!B251 &amp; """,name:""" &amp; CO!E251 &amp; """,x:" &amp; CO!G251&amp;"},"</f>
         <v>{id:1250,code:"YE",name:"Yemen",x:0},</v>
@@ -20729,7 +20729,7 @@
         <v>Mayotte</v>
       </c>
     </row>
-    <row r="253" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="str">
         <f>"{id:" &amp; CO!A253 &amp; ",code:""" &amp; CO!B253 &amp; """,name:""" &amp; CO!E253 &amp; """,x:" &amp; CO!G253&amp;"},"</f>
         <v>{id:1252,code:"ZA",name:"Sudáfrica",x:0},</v>
@@ -20743,7 +20743,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="str">
         <f>"{id:" &amp; CO!A254 &amp; ",code:""" &amp; CO!B254 &amp; """,name:""" &amp; CO!E254 &amp; """,x:" &amp; CO!G254&amp;"},"</f>
         <v>{id:1253,code:"ZM",name:"Zambia",x:0},</v>
@@ -20757,7 +20757,7 @@
         <v>Zambia</v>
       </c>
     </row>
-    <row r="255" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="str">
         <f>"{id:" &amp; CO!A255 &amp; ",code:""" &amp; CO!B255 &amp; """,name:""" &amp; CO!E255 &amp; """,x:" &amp; CO!G255&amp;"},"</f>
         <v>{id:1254,code:"ZW",name:"Zimbabue",x:0},</v>
@@ -20775,7 +20775,11 @@
   <autoFilter ref="A1:C255">
     <filterColumn colId="1">
       <filters>
+        <filter val="AFRICA"/>
         <filter val="AMERICA"/>
+        <filter val="ANTARTICA"/>
+        <filter val="ASIA"/>
+        <filter val="EUROPA"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:C255">

</xml_diff>

<commit_message>
fixed flags, select first flag if none selected
</commit_message>
<xml_diff>
--- a/docs/flags.xlsx
+++ b/docs/flags.xlsx
@@ -3982,12 +3982,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I142" sqref="I142"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4031,7 +4030,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4060,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4089,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -4147,7 +4146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -4176,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4234,7 +4233,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4321,7 +4320,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>386</v>
       </c>
@@ -4379,7 +4378,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -4437,7 +4436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -4466,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -4524,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -4582,7 +4581,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -4611,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -4698,7 +4697,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -4727,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -4756,7 +4755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -4785,7 +4784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>292</v>
       </c>
@@ -4843,7 +4842,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -4872,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -4930,7 +4929,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -4959,7 +4958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4988,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -5017,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -5046,7 +5045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>232</v>
       </c>
@@ -5104,7 +5103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -5162,7 +5161,7 @@
         <v>-24</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>431</v>
       </c>
@@ -5220,7 +5219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>93</v>
       </c>
@@ -5249,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>106</v>
       </c>
@@ -5278,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>474</v>
       </c>
@@ -5336,7 +5335,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>236</v>
       </c>
@@ -5365,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -5394,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -5423,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>240</v>
       </c>
@@ -5452,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>243</v>
       </c>
@@ -5481,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -5539,7 +5538,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>193</v>
       </c>
@@ -5597,7 +5596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>114</v>
       </c>
@@ -5684,7 +5683,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>126</v>
       </c>
@@ -5742,7 +5741,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -5771,7 +5770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>130</v>
       </c>
@@ -5800,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>405</v>
       </c>
@@ -5829,7 +5828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>401</v>
       </c>
@@ -5858,7 +5857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>132</v>
       </c>
@@ -5916,7 +5915,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -5945,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -5974,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>354</v>
       </c>
@@ -6003,7 +6002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -6032,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -6061,7 +6060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -6090,7 +6089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -6119,7 +6118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>167</v>
       </c>
@@ -6148,7 +6147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>155</v>
       </c>
@@ -6177,7 +6176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>161</v>
       </c>
@@ -6206,7 +6205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>163</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -6432,7 +6431,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>159</v>
       </c>
@@ -6458,7 +6457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>169</v>
       </c>
@@ -6487,7 +6486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>173</v>
       </c>
@@ -6516,7 +6515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>183</v>
       </c>
@@ -6632,7 +6631,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>187</v>
       </c>
@@ -6661,7 +6660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>197</v>
       </c>
@@ -6690,7 +6689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>207</v>
       </c>
@@ -6719,7 +6718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>199</v>
       </c>
@@ -6748,7 +6747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>213</v>
       </c>
@@ -6777,7 +6776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>211</v>
       </c>
@@ -6806,7 +6805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>201</v>
       </c>
@@ -6835,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>66</v>
       </c>
@@ -6861,7 +6860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>205</v>
       </c>
@@ -6890,7 +6889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>104</v>
       </c>
@@ -6919,7 +6918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>326</v>
       </c>
@@ -6945,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>216</v>
       </c>
@@ -7032,7 +7031,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>76</v>
       </c>
@@ -7061,7 +7060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>87</v>
       </c>
@@ -7090,7 +7089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>28</v>
       </c>
@@ -7116,7 +7115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>145</v>
       </c>
@@ -7145,7 +7144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>177</v>
       </c>
@@ -7171,7 +7170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>189</v>
       </c>
@@ -7255,7 +7254,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>298</v>
       </c>
@@ -7284,7 +7283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>285</v>
       </c>
@@ -7313,7 +7312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>362</v>
       </c>
@@ -7342,7 +7341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>388</v>
       </c>
@@ -7400,7 +7399,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>466</v>
       </c>
@@ -7426,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>481</v>
       </c>
@@ -7484,7 +7483,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>203</v>
       </c>
@@ -7513,7 +7512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>218</v>
       </c>
@@ -7571,7 +7570,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>226</v>
       </c>
@@ -7600,7 +7599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>220</v>
       </c>
@@ -7626,7 +7625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>224</v>
       </c>
@@ -7655,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>249</v>
       </c>
@@ -7684,7 +7683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>228</v>
       </c>
@@ -7713,7 +7712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>230</v>
       </c>
@@ -7742,7 +7741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>234</v>
       </c>
@@ -7771,7 +7770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>245</v>
       </c>
@@ -7800,7 +7799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>253</v>
       </c>
@@ -7829,7 +7828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>251</v>
       </c>
@@ -7858,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>263</v>
       </c>
@@ -7887,7 +7886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>269</v>
       </c>
@@ -7916,7 +7915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>261</v>
       </c>
@@ -7945,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>271</v>
       </c>
@@ -7974,7 +7973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>257</v>
       </c>
@@ -8003,7 +8002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>265</v>
       </c>
@@ -8032,7 +8031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>267</v>
       </c>
@@ -8090,7 +8089,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>275</v>
       </c>
@@ -8119,7 +8118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>296</v>
       </c>
@@ -8148,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>287</v>
       </c>
@@ -8177,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>283</v>
       </c>
@@ -8206,7 +8205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>316</v>
       </c>
@@ -8235,7 +8234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>312</v>
       </c>
@@ -8264,7 +8263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>290</v>
       </c>
@@ -8293,7 +8292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>306</v>
       </c>
@@ -8322,7 +8321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>273</v>
       </c>
@@ -8351,7 +8350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>300</v>
       </c>
@@ -8377,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>308</v>
       </c>
@@ -8406,7 +8405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>302</v>
       </c>
@@ -8435,7 +8434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>498</v>
       </c>
@@ -8464,7 +8463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>142</v>
       </c>
@@ -8493,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>277</v>
       </c>
@@ -8522,7 +8521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>294</v>
       </c>
@@ -8551,7 +8550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>279</v>
       </c>
@@ -8609,7 +8608,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>318</v>
       </c>
@@ -8638,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>320</v>
       </c>
@@ -8667,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>338</v>
       </c>
@@ -8696,7 +8695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>336</v>
       </c>
@@ -8754,7 +8753,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>324</v>
       </c>
@@ -8783,7 +8782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>328</v>
       </c>
@@ -8812,7 +8811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>340</v>
       </c>
@@ -8841,7 +8840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>334</v>
       </c>
@@ -8870,7 +8869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>322</v>
       </c>
@@ -8899,7 +8898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>342</v>
       </c>
@@ -8928,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>344</v>
       </c>
@@ -8957,7 +8956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>332</v>
       </c>
@@ -8986,7 +8985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -9015,7 +9014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>370</v>
       </c>
@@ -9044,7 +9043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>366</v>
       </c>
@@ -9099,7 +9098,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>352</v>
       </c>
@@ -9186,7 +9185,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>350</v>
       </c>
@@ -9215,7 +9214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>358</v>
       </c>
@@ -9244,7 +9243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>368</v>
       </c>
@@ -9302,7 +9301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>374</v>
       </c>
@@ -9331,7 +9330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>151</v>
       </c>
@@ -9360,7 +9359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>81</v>
       </c>
@@ -9389,7 +9388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>108</v>
       </c>
@@ -9447,7 +9446,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>376</v>
       </c>
@@ -9473,7 +9472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>384</v>
       </c>
@@ -9502,7 +9501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>378</v>
       </c>
@@ -9531,7 +9530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>382</v>
       </c>
@@ -9560,7 +9559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>128</v>
       </c>
@@ -9586,7 +9585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>494</v>
       </c>
@@ -9615,7 +9614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>20</v>
       </c>
@@ -9702,7 +9701,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>409</v>
       </c>
@@ -9818,7 +9817,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>398</v>
       </c>
@@ -9876,7 +9875,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>419</v>
       </c>
@@ -9905,7 +9904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>411</v>
       </c>
@@ -9934,7 +9933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>380</v>
       </c>
@@ -9963,7 +9962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>390</v>
       </c>
@@ -9992,7 +9991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>407</v>
       </c>
@@ -10021,7 +10020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>396</v>
       </c>
@@ -10050,7 +10049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>425</v>
       </c>
@@ -10079,7 +10078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>413</v>
       </c>
@@ -10108,7 +10107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>259</v>
       </c>
@@ -10137,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>500</v>
       </c>
@@ -10166,7 +10165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>392</v>
       </c>
@@ -10195,7 +10194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>394</v>
       </c>
@@ -10224,7 +10223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>84</v>
       </c>
@@ -10253,7 +10252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>415</v>
       </c>
@@ -10282,7 +10281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>403</v>
       </c>
@@ -10308,7 +10307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>427</v>
       </c>
@@ -10337,7 +10336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>439</v>
       </c>
@@ -10366,7 +10365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>437</v>
       </c>
@@ -10395,7 +10394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>457</v>
       </c>
@@ -10424,7 +10423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>459</v>
       </c>
@@ -10453,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>209</v>
       </c>
@@ -10479,7 +10478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>433</v>
       </c>
@@ -10505,7 +10504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>443</v>
       </c>
@@ -10534,7 +10533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>435</v>
       </c>
@@ -10563,7 +10562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>441</v>
       </c>
@@ -10592,7 +10591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>449</v>
       </c>
@@ -10650,7 +10649,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>447</v>
       </c>
@@ -10679,7 +10678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>445</v>
       </c>
@@ -10708,7 +10707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>451</v>
       </c>
@@ -10737,7 +10736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>455</v>
       </c>
@@ -10766,7 +10765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>462</v>
       </c>
@@ -10795,7 +10794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>464</v>
       </c>
@@ -10853,7 +10852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>472</v>
       </c>
@@ -10882,7 +10881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>488</v>
       </c>
@@ -10940,7 +10939,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>486</v>
       </c>
@@ -10969,7 +10968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>490</v>
       </c>
@@ -10998,7 +10997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>496</v>
       </c>
@@ -11027,7 +11026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>112</v>
       </c>
@@ -11056,7 +11055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>502</v>
       </c>
@@ -11085,7 +11084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>504</v>
       </c>
@@ -11151,7 +11150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>511</v>
       </c>
@@ -11165,7 +11164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>513</v>
       </c>
@@ -11179,7 +11178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>515</v>
       </c>
@@ -11193,7 +11192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>517</v>
       </c>
@@ -11207,7 +11206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>417</v>
       </c>
@@ -11235,7 +11234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>492</v>
       </c>
@@ -11250,13 +11249,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I256">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="AMERICA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I256"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -11266,8 +11259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G255"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17194,9 +17187,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A255"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17215,7 +17206,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>"{id:" &amp; CO!A2 &amp; ",code:""" &amp; CO!B2 &amp; """,name:""" &amp; CO!E2 &amp; """,x:" &amp; CO!G2&amp;"},"</f>
         <v>{id:1001,code:"AD",name:"Andorra",x:0},</v>
@@ -17285,7 +17276,7 @@
         <v>Anguilla</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>"{id:" &amp; CO!A7 &amp; ",code:""" &amp; CO!B7 &amp; """,name:""" &amp; CO!E7 &amp; """,x:" &amp; CO!G7&amp;"},"</f>
         <v>{id:1006,code:"AL",name:"Albania",x:0},</v>
@@ -17327,7 +17318,7 @@
         <v>Angola</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>"{id:" &amp; CO!A10 &amp; ",code:""" &amp; CO!B10 &amp; """,name:""" &amp; CO!E10 &amp; """,x:" &amp; CO!G10&amp;"},"</f>
         <v>{id:1009,code:"AQ",name:"Antártida",x:0},</v>
@@ -17369,7 +17360,7 @@
         <v>American Samoa</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>"{id:" &amp; CO!A13 &amp; ",code:""" &amp; CO!B13 &amp; """,name:""" &amp; CO!E13 &amp; """,x:" &amp; CO!G13&amp;"},"</f>
         <v>{id:1012,code:"AT",name:"Austria",x:0},</v>
@@ -17383,7 +17374,7 @@
         <v>Austria</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>"{id:" &amp; CO!A14 &amp; ",code:""" &amp; CO!B14 &amp; """,name:""" &amp; CO!E14 &amp; """,x:" &amp; CO!G14&amp;"},"</f>
         <v>{id:1013,code:"AU",name:"Australia",x:0},</v>
@@ -17439,7 +17430,7 @@
         <v>Azerbaijan</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>"{id:" &amp; CO!A18 &amp; ",code:""" &amp; CO!B18 &amp; """,name:""" &amp; CO!E18 &amp; """,x:" &amp; CO!G18&amp;"},"</f>
         <v>{id:1017,code:"BA",name:"Bosnia y Herzegovina",x:0},</v>
@@ -17481,7 +17472,7 @@
         <v>Bangladesh</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>"{id:" &amp; CO!A21 &amp; ",code:""" &amp; CO!B21 &amp; """,name:""" &amp; CO!E21 &amp; """,x:" &amp; CO!G21&amp;"},"</f>
         <v>{id:1020,code:"BE",name:"Bélgica",x:0},</v>
@@ -17509,7 +17500,7 @@
         <v>Burkina Faso</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>"{id:" &amp; CO!A23 &amp; ",code:""" &amp; CO!B23 &amp; """,name:""" &amp; CO!E23 &amp; """,x:" &amp; CO!G23&amp;"},"</f>
         <v>{id:1022,code:"BG",name:"Bulgaria",x:0},</v>
@@ -17705,7 +17696,7 @@
         <v>Botswana</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>"{id:" &amp; CO!A37 &amp; ",code:""" &amp; CO!B37 &amp; """,name:""" &amp; CO!E37 &amp; """,x:" &amp; CO!G37&amp;"},"</f>
         <v>{id:1036,code:"BY",name:"Bielorrusia",x:0},</v>
@@ -17803,7 +17794,7 @@
         <v>Congo</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>"{id:" &amp; CO!A44 &amp; ",code:""" &amp; CO!B44 &amp; """,name:""" &amp; CO!E44 &amp; """,x:" &amp; CO!G44&amp;"},"</f>
         <v>{id:1043,code:"CH",name:"Suiza",x:0},</v>
@@ -17971,7 +17962,7 @@
         <v>Christmas Island</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>"{id:" &amp; CO!A56 &amp; ",code:""" &amp; CO!B56 &amp; """,name:""" &amp; CO!E56 &amp; """,x:" &amp; CO!G56&amp;"},"</f>
         <v>{id:1055,code:"CY",name:"Chipre",x:0},</v>
@@ -17985,7 +17976,7 @@
         <v>Cyprus</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>"{id:" &amp; CO!A57 &amp; ",code:""" &amp; CO!B57 &amp; """,name:""" &amp; CO!E57 &amp; """,x:" &amp; CO!G57&amp;"},"</f>
         <v>{id:1056,code:"CZ",name:"República Checa",x:0},</v>
@@ -17999,7 +17990,7 @@
         <v>Czech Republic</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>"{id:" &amp; CO!A58 &amp; ",code:""" &amp; CO!B58 &amp; """,name:""" &amp; CO!E58 &amp; """,x:" &amp; CO!G58&amp;"},"</f>
         <v>{id:1057,code:"DE",name:"Alemania",x:0},</v>
@@ -18027,7 +18018,7 @@
         <v>Djibouti</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>"{id:" &amp; CO!A60 &amp; ",code:""" &amp; CO!B60 &amp; """,name:""" &amp; CO!E60 &amp; """,x:" &amp; CO!G60&amp;"},"</f>
         <v>{id:1059,code:"DK",name:"Dinamarca",x:0},</v>
@@ -18097,7 +18088,7 @@
         <v>Ecuador</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>"{id:" &amp; CO!A65 &amp; ",code:""" &amp; CO!B65 &amp; """,name:""" &amp; CO!E65 &amp; """,x:" &amp; CO!G65&amp;"},"</f>
         <v>{id:1064,code:"EE",name:"Estonia",x:0},</v>
@@ -18153,7 +18144,7 @@
         <v>Eritrea</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>"{id:" &amp; CO!A69 &amp; ",code:""" &amp; CO!B69 &amp; """,name:""" &amp; CO!E69 &amp; """,x:" &amp; CO!G69&amp;"},"</f>
         <v>{id:1068,code:"ES",name:"España",x:0},</v>
@@ -18181,7 +18172,7 @@
         <v>Ethiopia</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>"{id:" &amp; CO!A71 &amp; ",code:""" &amp; CO!B71 &amp; """,name:""" &amp; CO!E71 &amp; """,x:" &amp; CO!G71&amp;"},"</f>
         <v>{id:1070,code:"FI",name:"Finlandia",x:0},</v>
@@ -18195,7 +18186,7 @@
         <v>Finland</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>"{id:" &amp; CO!A72 &amp; ",code:""" &amp; CO!B72 &amp; """,name:""" &amp; CO!E72 &amp; """,x:" &amp; CO!G72&amp;"},"</f>
         <v>{id:1071,code:"FJ",name:"Fiyi",x:0},</v>
@@ -18223,7 +18214,7 @@
         <v>Falkland Islands (Malvinas)</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>"{id:" &amp; CO!A74 &amp; ",code:""" &amp; CO!B74 &amp; """,name:""" &amp; CO!E74 &amp; """,x:" &amp; CO!G74&amp;"},"</f>
         <v>{id:1073,code:"FM",name:"Micronesia",x:0},</v>
@@ -18251,7 +18242,7 @@
         <v>Faroe Islands</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>"{id:" &amp; CO!A76 &amp; ",code:""" &amp; CO!B76 &amp; """,name:""" &amp; CO!E76 &amp; """,x:" &amp; CO!G76&amp;"},"</f>
         <v>{id:1075,code:"FR",name:"Francia",x:0},</v>
@@ -18335,7 +18326,7 @@
         <v>Wales</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f>"{id:" &amp; CO!A82 &amp; ",code:""" &amp; CO!B82 &amp; """,name:""" &amp; CO!E82 &amp; """,x:" &amp; CO!G82&amp;"},"</f>
         <v>{id:1081,code:"GB",name:"Reino Unido",x:0},</v>
@@ -18391,7 +18382,7 @@
         <v>French Guiana</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>"{id:" &amp; CO!A86 &amp; ",code:""" &amp; CO!B86 &amp; """,name:""" &amp; CO!E86 &amp; """,x:" &amp; CO!G86&amp;"},"</f>
         <v>{id:1085,code:"GG",name:"Guernsey",x:0},</v>
@@ -18503,7 +18494,7 @@
         <v>Equatorial Guinea</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f>"{id:" &amp; CO!A94 &amp; ",code:""" &amp; CO!B94 &amp; """,name:""" &amp; CO!E94 &amp; """,x:" &amp; CO!G94&amp;"},"</f>
         <v>{id:1093,code:"GR",name:"Grecia",x:0},</v>
@@ -18629,7 +18620,7 @@
         <v>Honduras</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
         <f>"{id:" &amp; CO!A103 &amp; ",code:""" &amp; CO!B103 &amp; """,name:""" &amp; CO!E103 &amp; """,x:" &amp; CO!G103&amp;"},"</f>
         <v>{id:1102,code:"HR",name:"Croacia",x:0},</v>
@@ -18657,7 +18648,7 @@
         <v>Haiti</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
         <f>"{id:" &amp; CO!A105 &amp; ",code:""" &amp; CO!B105 &amp; """,name:""" &amp; CO!E105 &amp; """,x:" &amp; CO!G105&amp;"},"</f>
         <v>{id:1104,code:"HU",name:"Hungría",x:0},</v>
@@ -18685,7 +18676,7 @@
         <v>Indonesia</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
         <f>"{id:" &amp; CO!A107 &amp; ",code:""" &amp; CO!B107 &amp; """,name:""" &amp; CO!E107 &amp; """,x:" &amp; CO!G107&amp;"},"</f>
         <v>{id:1106,code:"IE",name:"Irlanda",x:0},</v>
@@ -18783,7 +18774,7 @@
         <v>Iran</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
         <f>"{id:" &amp; CO!A114 &amp; ",code:""" &amp; CO!B114 &amp; """,name:""" &amp; CO!E114 &amp; """,x:" &amp; CO!G114&amp;"},"</f>
         <v>{id:1113,code:"IS",name:"Islandia",x:0},</v>
@@ -18797,7 +18788,7 @@
         <v>Iceland</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
         <f>"{id:" &amp; CO!A115 &amp; ",code:""" &amp; CO!B115 &amp; """,name:""" &amp; CO!E115 &amp; """,x:" &amp; CO!G115&amp;"},"</f>
         <v>{id:1114,code:"IT",name:"Italia",x:0},</v>
@@ -18909,7 +18900,7 @@
         <v>Cambodia</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
         <f>"{id:" &amp; CO!A123 &amp; ",code:""" &amp; CO!B123 &amp; """,name:""" &amp; CO!E123 &amp; """,x:" &amp; CO!G123&amp;"},"</f>
         <v>{id:1122,code:"KI",name:"Kiribati",x:0},</v>
@@ -19063,7 +19054,7 @@
         <v>Saint Lucia</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f>"{id:" &amp; CO!A134 &amp; ",code:""" &amp; CO!B134 &amp; """,name:""" &amp; CO!E134 &amp; """,x:" &amp; CO!G134&amp;"},"</f>
         <v>{id:1133,code:"LI",name:"Liechtenstein",x:0},</v>
@@ -19119,7 +19110,7 @@
         <v>Lesotho</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
         <f>"{id:" &amp; CO!A138 &amp; ",code:""" &amp; CO!B138 &amp; """,name:""" &amp; CO!E138 &amp; """,x:" &amp; CO!G138&amp;"},"</f>
         <v>{id:1137,code:"LT",name:"Lituania",x:0},</v>
@@ -19133,7 +19124,7 @@
         <v>Lithuania</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
         <f>"{id:" &amp; CO!A139 &amp; ",code:""" &amp; CO!B139 &amp; """,name:""" &amp; CO!E139 &amp; """,x:" &amp; CO!G139&amp;"},"</f>
         <v>{id:1138,code:"LU",name:"Luxemburgo",x:0},</v>
@@ -19147,7 +19138,7 @@
         <v>Luxembourg</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
         <f>"{id:" &amp; CO!A140 &amp; ",code:""" &amp; CO!B140 &amp; """,name:""" &amp; CO!E140 &amp; """,x:" &amp; CO!G140&amp;"},"</f>
         <v>{id:1139,code:"LV",name:"Letonia",x:0},</v>
@@ -19189,7 +19180,7 @@
         <v>Morocco</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
         <f>"{id:" &amp; CO!A143 &amp; ",code:""" &amp; CO!B143 &amp; """,name:""" &amp; CO!E143 &amp; """,x:" &amp; CO!G143&amp;"},"</f>
         <v>{id:1142,code:"MC",name:"Mónaco",x:0},</v>
@@ -19203,7 +19194,7 @@
         <v>Monaco</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
         <f>"{id:" &amp; CO!A144 &amp; ",code:""" &amp; CO!B144 &amp; """,name:""" &amp; CO!E144 &amp; """,x:" &amp; CO!G144&amp;"},"</f>
         <v>{id:1143,code:"MD",name:"Moldavia",x:0},</v>
@@ -19217,7 +19208,7 @@
         <v>Moldova</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
         <f>"{id:" &amp; CO!A145 &amp; ",code:""" &amp; CO!B145 &amp; """,name:""" &amp; CO!E145 &amp; """,x:" &amp; CO!G145&amp;"},"</f>
         <v>{id:1144,code:"ME",name:"Montenegro",x:0},</v>
@@ -19259,7 +19250,7 @@
         <v>Madagascar</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
         <f>"{id:" &amp; CO!A148 &amp; ",code:""" &amp; CO!B148 &amp; """,name:""" &amp; CO!E148 &amp; """,x:" &amp; CO!G148&amp;"},"</f>
         <v>{id:1147,code:"MH",name:"Islas Marshall",x:0},</v>
@@ -19273,7 +19264,7 @@
         <v>Marshall Islands</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
         <f>"{id:" &amp; CO!A149 &amp; ",code:""" &amp; CO!B149 &amp; """,name:""" &amp; CO!E149 &amp; """,x:" &amp; CO!G149&amp;"},"</f>
         <v>{id:1148,code:"MK",name:"Macedónia",x:0},</v>
@@ -19399,7 +19390,7 @@
         <v>Montserrat</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="str">
         <f>"{id:" &amp; CO!A158 &amp; ",code:""" &amp; CO!B158 &amp; """,name:""" &amp; CO!E158 &amp; """,x:" &amp; CO!G158&amp;"},"</f>
         <v>{id:1157,code:"MT",name:"Malta",x:0},</v>
@@ -19581,7 +19572,7 @@
         <v>Nicaragua</v>
       </c>
     </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
         <f>"{id:" &amp; CO!A171 &amp; ",code:""" &amp; CO!B171 &amp; """,name:""" &amp; CO!E171 &amp; """,x:" &amp; CO!G171&amp;"},"</f>
         <v>{id:1170,code:"NL",name:"Países Bajos",x:0},</v>
@@ -19595,7 +19586,7 @@
         <v>Netherlands</v>
       </c>
     </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
         <f>"{id:" &amp; CO!A172 &amp; ",code:""" &amp; CO!B172 &amp; """,name:""" &amp; CO!E172 &amp; """,x:" &amp; CO!G172&amp;"},"</f>
         <v>{id:1171,code:"NO",name:"Noruega",x:0},</v>
@@ -19623,7 +19614,7 @@
         <v>Nepal</v>
       </c>
     </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
         <f>"{id:" &amp; CO!A174 &amp; ",code:""" &amp; CO!B174 &amp; """,name:""" &amp; CO!E174 &amp; """,x:" &amp; CO!G174&amp;"},"</f>
         <v>{id:1173,code:"NR",name:"Nauru",x:0},</v>
@@ -19651,7 +19642,7 @@
         <v>Niue</v>
       </c>
     </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
         <f>"{id:" &amp; CO!A176 &amp; ",code:""" &amp; CO!B176 &amp; """,name:""" &amp; CO!E176 &amp; """,x:" &amp; CO!G176&amp;"},"</f>
         <v>{id:1175,code:"NZ",name:"Nueva Zelanda",x:0},</v>
@@ -19721,7 +19712,7 @@
         <v>French Polynesia</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="str">
         <f>"{id:" &amp; CO!A181 &amp; ",code:""" &amp; CO!B181 &amp; """,name:""" &amp; CO!E181 &amp; """,x:" &amp; CO!G181&amp;"},"</f>
         <v>{id:1180,code:"PG",name:"Papúa Nueva Guinea",x:0},</v>
@@ -19763,7 +19754,7 @@
         <v>Pakistan</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="str">
         <f>"{id:" &amp; CO!A184 &amp; ",code:""" &amp; CO!B184 &amp; """,name:""" &amp; CO!E184 &amp; """,x:" &amp; CO!G184&amp;"},"</f>
         <v>{id:1183,code:"PL",name:"Polonia",x:0},</v>
@@ -19833,7 +19824,7 @@
         <v>Palestine</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="str">
         <f>"{id:" &amp; CO!A189 &amp; ",code:""" &amp; CO!B189 &amp; """,name:""" &amp; CO!E189 &amp; """,x:" &amp; CO!G189&amp;"},"</f>
         <v>{id:1188,code:"PT",name:"Portugal",x:0},</v>
@@ -19847,7 +19838,7 @@
         <v>Portugal</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="str">
         <f>"{id:" &amp; CO!A190 &amp; ",code:""" &amp; CO!B190 &amp; """,name:""" &amp; CO!E190 &amp; """,x:" &amp; CO!G190&amp;"},"</f>
         <v>{id:1189,code:"PW",name:"Palau",x:0},</v>
@@ -19903,7 +19894,7 @@
         <v>Réunion</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="str">
         <f>"{id:" &amp; CO!A194 &amp; ",code:""" &amp; CO!B194 &amp; """,name:""" &amp; CO!E194 &amp; """,x:" &amp; CO!G194&amp;"},"</f>
         <v>{id:1193,code:"RO",name:"Rumanía",x:0},</v>
@@ -19917,7 +19908,7 @@
         <v>Romania</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="str">
         <f>"{id:" &amp; CO!A195 &amp; ",code:""" &amp; CO!B195 &amp; """,name:""" &amp; CO!E195 &amp; """,x:" &amp; CO!G195&amp;"},"</f>
         <v>{id:1194,code:"RS",name:"Serbia",x:0},</v>
@@ -19973,7 +19964,7 @@
         <v>Saudi Arabia</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="str">
         <f>"{id:" &amp; CO!A199 &amp; ",code:""" &amp; CO!B199 &amp; """,name:""" &amp; CO!E199 &amp; """,x:" &amp; CO!G199&amp;"},"</f>
         <v>{id:1198,code:"SB",name:"Islas Salomón",x:0},</v>
@@ -20015,7 +20006,7 @@
         <v>Sudan</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="str">
         <f>"{id:" &amp; CO!A202 &amp; ",code:""" &amp; CO!B202 &amp; """,name:""" &amp; CO!E202 &amp; """,x:" &amp; CO!G202&amp;"},"</f>
         <v>{id:1201,code:"SE",name:"Suecia",x:0},</v>
@@ -20057,7 +20048,7 @@
         <v>Saint Helena</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="str">
         <f>"{id:" &amp; CO!A205 &amp; ",code:""" &amp; CO!B205 &amp; """,name:""" &amp; CO!E205 &amp; """,x:" &amp; CO!G205&amp;"},"</f>
         <v>{id:1204,code:"SI",name:"Eslovenia",x:0},</v>
@@ -20085,7 +20076,7 @@
         <v>Svalbard and Jan Mayen Islands</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="str">
         <f>"{id:" &amp; CO!A207 &amp; ",code:""" &amp; CO!B207 &amp; """,name:""" &amp; CO!E207 &amp; """,x:" &amp; CO!G207&amp;"},"</f>
         <v>{id:1206,code:"SK",name:"Eslovaquia",x:0},</v>
@@ -20113,7 +20104,7 @@
         <v>Sierra Leone</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="str">
         <f>"{id:" &amp; CO!A209 &amp; ",code:""" &amp; CO!B209 &amp; """,name:""" &amp; CO!E209 &amp; """,x:" &amp; CO!G209&amp;"},"</f>
         <v>{id:1208,code:"SM",name:"San Marino",x:0},</v>
@@ -20393,7 +20384,7 @@
         <v>Tunisia</v>
       </c>
     </row>
-    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="str">
         <f>"{id:" &amp; CO!A229 &amp; ",code:""" &amp; CO!B229 &amp; """,name:""" &amp; CO!E229 &amp; """,x:" &amp; CO!G229&amp;"},"</f>
         <v>{id:1228,code:"TO",name:"Tonga",x:0},</v>
@@ -20435,7 +20426,7 @@
         <v>Trinidad and Tobago</v>
       </c>
     </row>
-    <row r="232" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="str">
         <f>"{id:" &amp; CO!A232 &amp; ",code:""" &amp; CO!B232 &amp; """,name:""" &amp; CO!E232 &amp; """,x:" &amp; CO!G232&amp;"},"</f>
         <v>{id:1231,code:"TV",name:"Tuvalu",x:0},</v>
@@ -20477,7 +20468,7 @@
         <v>Tanzania</v>
       </c>
     </row>
-    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="str">
         <f>"{id:" &amp; CO!A235 &amp; ",code:""" &amp; CO!B235 &amp; """,name:""" &amp; CO!E235 &amp; """,x:" &amp; CO!G235&amp;"},"</f>
         <v>{id:1234,code:"UA",name:"Ucrania",x:0},</v>
@@ -20561,7 +20552,7 @@
         <v>Uzbekistan</v>
       </c>
     </row>
-    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="str">
         <f>"{id:" &amp; CO!A241 &amp; ",code:""" &amp; CO!B241 &amp; """,name:""" &amp; CO!E241 &amp; """,x:" &amp; CO!G241&amp;"},"</f>
         <v>{id:1240,code:"VA",name:"Ciudad del Vaticano",x:0},</v>
@@ -20645,7 +20636,7 @@
         <v>Viet Nam</v>
       </c>
     </row>
-    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="str">
         <f>"{id:" &amp; CO!A247 &amp; ",code:""" &amp; CO!B247 &amp; """,name:""" &amp; CO!E247 &amp; """,x:" &amp; CO!G247&amp;"},"</f>
         <v>{id:1246,code:"VU",name:"Vanuatu",x:0},</v>
@@ -20687,7 +20678,7 @@
         <v>Kosovo</v>
       </c>
     </row>
-    <row r="250" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="str">
         <f>"{id:" &amp; CO!A250 &amp; ",code:""" &amp; CO!B250 &amp; """,name:""" &amp; CO!E250 &amp; """,x:" &amp; CO!G250&amp;"},"</f>
         <v>{id:1249,code:"WS",name:"Samoa",x:0},</v>
@@ -20777,9 +20768,9 @@
       <filters>
         <filter val="AFRICA"/>
         <filter val="AMERICA"/>
-        <filter val="ANTARTICA"/>
         <filter val="ASIA"/>
         <filter val="EUROPA"/>
+        <filter val="OCEANIA"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:C255">
@@ -20794,7 +20785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A255"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -22336,9 +22327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>